<commit_message>
Fix Table Estado Equipo
Se arregla error de la tabla Estado de equipo, la cual hacia division de estados segun la unidad asignada
</commit_message>
<xml_diff>
--- a/Flask/app/datos_exportados.xlsx
+++ b/Flask/app/datos_exportados.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,348 +497,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>San Pedro de la Paz</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Jardin Nueva Vida</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Notebook</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Acer</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Nitro 5</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>San Pedro de la Paz</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Jardin Nueva Vida</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Impresora</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Epson</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>L390</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>San Pedro de la Paz</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Jardin Nueva Vida</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Impresora</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Epson</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>L390</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>San Pedro de la Paz</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Jardin Nueva Vida</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Notebook</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Asus</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">aspire </t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Jardin Conce</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Monitor</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>LG</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>G27</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Jardin Conce</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Telefono</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Samsung</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>A55</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>